<commit_message>
Add total fertlity rate in Germany visualization
</commit_message>
<xml_diff>
--- a/data/Armutsgefaehrdungsquote-nach-Haushaltstyp.xlsx
+++ b/data/Armutsgefaehrdungsquote-nach-Haushaltstyp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee98f7950f31f1d/Desktop/Clemens Policy Paper/graphs/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ee98f7950f31f1d/50-59 Personal/54 Portfolio/54.01 Policy Paper Graphs/demographic-change-germany/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{F548DD34-BE3E-4730-B222-38949BC0D6E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8CFD9192-1798-464F-BDFB-6A39CD2A5556}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{F548DD34-BE3E-4730-B222-38949BC0D6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CFD9192-1798-464F-BDFB-6A39CD2A5556}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21465" windowHeight="17685" xr2:uid="{8EBD7ACA-2C39-4CC9-8B9A-A87F2545816C}"/>
+    <workbookView xWindow="11550" yWindow="4215" windowWidth="23295" windowHeight="14415" xr2:uid="{8EBD7ACA-2C39-4CC9-8B9A-A87F2545816C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -444,9 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9698B5-3B71-42D1-B9A7-BF4040CDD76A}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:I18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>